<commit_message>
Ready to start layout
</commit_message>
<xml_diff>
--- a/Hardware/NFC Toy BOM.xlsx
+++ b/Hardware/NFC Toy BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="102">
   <si>
     <t>Part #</t>
   </si>
@@ -173,12 +173,6 @@
     <t>For J-Link</t>
   </si>
   <si>
-    <t>STM32F051K8T6</t>
-  </si>
-  <si>
-    <t>Cortex-M0, 64 kB flash</t>
-  </si>
-  <si>
     <t>32-LQFP</t>
   </si>
   <si>
@@ -188,15 +182,6 @@
     <t xml:space="preserve">3xSPI/I2S. 1 DAC. </t>
   </si>
   <si>
-    <t>TMP102AIDRLR</t>
-  </si>
-  <si>
-    <t>I2C Temp Sensor</t>
-  </si>
-  <si>
-    <t>SOT-563</t>
-  </si>
-  <si>
     <t>Lite-On</t>
   </si>
   <si>
@@ -245,26 +230,117 @@
     <t>4-SMD</t>
   </si>
   <si>
-    <t>SN74LVC1T45</t>
-  </si>
-  <si>
     <t>Dual Level Translator</t>
   </si>
   <si>
-    <t>SOT-23-6</t>
-  </si>
-  <si>
     <t>For dotstar</t>
+  </si>
+  <si>
+    <t>SN74LVC2T45</t>
+  </si>
+  <si>
+    <t>8-VSSOP</t>
+  </si>
+  <si>
+    <t>Capacitor - 0.1uF</t>
+  </si>
+  <si>
+    <t>Capacitor - 10uF</t>
+  </si>
+  <si>
+    <t>Capacitor - 2.2uF</t>
+  </si>
+  <si>
+    <t>Capacitor - 1uF</t>
+  </si>
+  <si>
+    <t>Capacitor (Tantalum) - 220uF</t>
+  </si>
+  <si>
+    <t>Capacitor - 33pF</t>
+  </si>
+  <si>
+    <t>Capacitor - 1000pF</t>
+  </si>
+  <si>
+    <t>Capacitor - 220pF</t>
+  </si>
+  <si>
+    <t>Capacitor - 22pF</t>
+  </si>
+  <si>
+    <t>Capacitor - 100pF</t>
+  </si>
+  <si>
+    <t>Inductor - 560 nH</t>
+  </si>
+  <si>
+    <t>Resistor - 121 ohm</t>
+  </si>
+  <si>
+    <t>Resistor - 10k ohm</t>
+  </si>
+  <si>
+    <t>Resistor - 30k ohm</t>
+  </si>
+  <si>
+    <t>Resistor - 1k ohm</t>
+  </si>
+  <si>
+    <t>Resistor - 1.5k ohm</t>
+  </si>
+  <si>
+    <t>Resistor - 1.6k ohm</t>
+  </si>
+  <si>
+    <t>MCT06030C1002FP500</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>RC0603FR-0730KL</t>
+  </si>
+  <si>
+    <t>RC0603FR-071KL</t>
+  </si>
+  <si>
+    <t>RC0603FR-071K5L</t>
+  </si>
+  <si>
+    <t>RC0603FR-071K6L</t>
+  </si>
+  <si>
+    <t>RMCF0603FT121R</t>
+  </si>
+  <si>
+    <t>Stackpole</t>
+  </si>
+  <si>
+    <t>MLJ1608WR56JT000</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>F950G227MAAAQ2</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Order Qty</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +355,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -298,15 +388,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -325,8 +413,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -639,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,12 +758,13 @@
     <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="3"/>
-    <col min="5" max="5" width="14.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="60.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="12"/>
+    <col min="6" max="6" width="14.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="60.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -665,16 +774,18 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -683,28 +794,32 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>68</v>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="2">
+        <v>50</v>
+      </c>
+      <c r="D2" s="10">
+        <v>1</v>
+      </c>
+      <c r="E2" s="12">
         <v>3.63</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" t="s">
         <v>51</v>
       </c>
-      <c r="F2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -714,17 +829,20 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="10">
+        <v>1</v>
+      </c>
+      <c r="E3" s="12">
         <v>2.2200000000000002</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -734,17 +852,20 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12">
         <v>11.99</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -754,18 +875,21 @@
       <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="10">
+        <v>1</v>
+      </c>
+      <c r="E5" s="12">
         <v>1.53</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
         <v>5031821852</v>
       </c>
       <c r="B6" t="s">
@@ -774,16 +898,19 @@
       <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="10">
+        <v>1</v>
+      </c>
+      <c r="E6" s="12">
         <v>2.33</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>67</v>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
@@ -791,18 +918,21 @@
       <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="10">
+        <v>1</v>
+      </c>
+      <c r="E7" s="12">
         <v>2.76</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B8" t="s">
@@ -811,15 +941,18 @@
       <c r="C8" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="10">
+        <v>1</v>
+      </c>
+      <c r="E8" s="12">
         <v>0.41</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
         <v>2343</v>
       </c>
       <c r="B9" t="s">
@@ -828,18 +961,21 @@
       <c r="C9" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="2">
-        <v>4.5</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="D9" s="10">
+        <v>2</v>
+      </c>
+      <c r="E9" s="12">
+        <v>9</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B10" t="s">
@@ -848,18 +984,21 @@
       <c r="C10" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="12">
         <v>1.29</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B11" t="s">
@@ -868,18 +1007,21 @@
       <c r="C11" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="10">
+        <v>1</v>
+      </c>
+      <c r="E11" s="12">
         <v>20.350000000000001</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>45</v>
       </c>
       <c r="B12" t="s">
@@ -888,173 +1030,399 @@
       <c r="C12" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="10">
+        <v>1</v>
+      </c>
+      <c r="E12" s="12">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>49</v>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="2">
-        <v>2.74</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="D13" s="10">
+        <v>1</v>
+      </c>
+      <c r="E13" s="12">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="2">
-        <v>2</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1</v>
+      </c>
+      <c r="E14" s="12">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" t="s">
         <v>59</v>
-      </c>
-      <c r="B15" t="s">
-        <v>57</v>
       </c>
       <c r="C15" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="2">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="D15" s="10">
+        <v>1</v>
+      </c>
+      <c r="E15" s="12">
+        <v>1.41</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>61</v>
       </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>63</v>
+        <v>66</v>
+      </c>
+      <c r="D16" s="10">
+        <v>1</v>
+      </c>
+      <c r="E16" s="12">
+        <v>1</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="2">
-        <v>1.41</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="10">
+        <v>1</v>
+      </c>
+      <c r="E17" s="12">
+        <v>0.61</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" t="s">
         <v>69</v>
       </c>
-      <c r="B18" t="s">
-        <v>70</v>
-      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" s="2">
-        <v>1</v>
-      </c>
-      <c r="E18" s="8" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="D18" s="10">
+        <v>20</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
         <v>73</v>
       </c>
-      <c r="B19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" s="10">
+        <v>10</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="E19" s="5" t="s">
+      <c r="D20" s="10">
+        <v>10</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>75</v>
       </c>
-      <c r="F19" t="s">
+      <c r="D21" s="10">
+        <v>10</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E30" s="5"/>
+      <c r="D22" s="10">
+        <v>2</v>
+      </c>
+      <c r="E22" s="12">
+        <v>2.12</v>
+      </c>
+      <c r="F22" s="4">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="10">
+        <v>10</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="10">
+        <v>10</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="10">
+        <v>10</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="10">
+        <v>10</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="10">
+        <v>10</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="10">
+        <v>4</v>
+      </c>
+      <c r="E28" s="12">
+        <v>1.2</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="10">
+        <v>10</v>
+      </c>
+      <c r="E29" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="10">
+        <v>20</v>
+      </c>
+      <c r="E30" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="10">
+        <v>10</v>
+      </c>
+      <c r="E31" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" s="10">
+        <v>10</v>
+      </c>
+      <c r="E32" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="10">
+        <v>10</v>
+      </c>
+      <c r="E33" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="10">
+        <v>10</v>
+      </c>
+      <c r="E34" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C38" s="14"/>
+      <c r="D38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E38" s="12">
+        <f>SUM(E2:E34)</f>
+        <v>64.580000000000013</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A30" r:id="rId1" display="https://www.digikey.com/product-detail/en/vishay-beyschlag/MCT06030C1002FP500/MCT0603-10.0K-CFCT-ND/2607933"/>
+    <hyperlink ref="A32" r:id="rId2" display="https://www.digikey.com/product-detail/en/yageo/RC0603FR-071KL/311-1.00KHRCT-ND/729790"/>
+    <hyperlink ref="A33" r:id="rId3" display="https://www.digikey.com/product-detail/en/yageo/RC0603FR-071K5L/311-1.50KHRCT-ND/729811"/>
+    <hyperlink ref="A34" r:id="rId4" display="https://www.digikey.com/product-detail/en/yageo/RC0603FR-071K6L/311-1.60KHRCT-ND/729815"/>
+    <hyperlink ref="A29" r:id="rId5" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RMCF0603FT121R/RMCF0603FT121RCT-ND/1942968"/>
+    <hyperlink ref="A28" r:id="rId6" display="https://www.digikey.com/product-detail/en/tdk-corporation/MLJ1608WR56JT000/445-174193-1-ND/5813302"/>
+    <hyperlink ref="A22" r:id="rId7" display="https://www.digikey.com/product-detail/en/avx-corporation/F950G227MAAAQ2/478-8368-1-ND/4005666"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
First pass layout complete
</commit_message>
<xml_diff>
--- a/Hardware/NFC Toy BOM.xlsx
+++ b/Hardware/NFC Toy BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="121">
   <si>
     <t>Part #</t>
   </si>
@@ -173,9 +173,6 @@
     <t>For J-Link</t>
   </si>
   <si>
-    <t>32-LQFP</t>
-  </si>
-  <si>
     <t>Cortex-M0+, 64kB flash, 64kB RAM</t>
   </si>
   <si>
@@ -215,9 +212,6 @@
     <t>TPS61032</t>
   </si>
   <si>
-    <t>STM32L052K8T6</t>
-  </si>
-  <si>
     <t>7M-27.120MAAJ-T</t>
   </si>
   <si>
@@ -384,6 +378,15 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Resistor - 0 ohm</t>
+  </si>
+  <si>
+    <t>STM32L052C8T6</t>
+  </si>
+  <si>
+    <t>48-LQFP</t>
   </si>
 </sst>
 </file>
@@ -805,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,7 +835,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>3</v>
@@ -844,7 +847,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -857,28 +860,28 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>63</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="10">
+        <v>1</v>
+      </c>
+      <c r="E2" s="12">
+        <v>3.77</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="10">
-        <v>1</v>
-      </c>
-      <c r="E2" s="12">
-        <v>3.63</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" t="s">
-        <v>51</v>
-      </c>
       <c r="H2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -904,7 +907,7 @@
         <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -930,7 +933,7 @@
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -956,7 +959,7 @@
         <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -979,12 +982,12 @@
         <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
@@ -1005,7 +1008,7 @@
         <v>26</v>
       </c>
       <c r="H7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1028,7 +1031,7 @@
         <v>30</v>
       </c>
       <c r="H8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1054,7 +1057,7 @@
         <v>32</v>
       </c>
       <c r="H9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1080,7 +1083,7 @@
         <v>37</v>
       </c>
       <c r="H10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1137,13 +1140,13 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" t="s">
         <v>54</v>
-      </c>
-      <c r="B13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" t="s">
-        <v>55</v>
       </c>
       <c r="D13" s="10">
         <v>1</v>
@@ -1152,7 +1155,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H13" t="s">
         <v>41</v>
@@ -1160,13 +1163,13 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
         <v>56</v>
-      </c>
-      <c r="B14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" t="s">
-        <v>57</v>
       </c>
       <c r="D14" s="10">
         <v>1</v>
@@ -1175,7 +1178,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H14" t="s">
         <v>41</v>
@@ -1183,13 +1186,13 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
         <v>58</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>59</v>
-      </c>
-      <c r="C15" t="s">
-        <v>60</v>
       </c>
       <c r="D15" s="10">
         <v>1</v>
@@ -1198,44 +1201,44 @@
         <v>1.41</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
         <v>64</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" s="10">
+        <v>1</v>
+      </c>
+      <c r="E16" s="12">
+        <v>1</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C16" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="10">
-        <v>1</v>
-      </c>
-      <c r="E16" s="12">
-        <v>1</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>67</v>
-      </c>
       <c r="H16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D17" s="10">
         <v>1</v>
@@ -1244,24 +1247,24 @@
         <v>0.61</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H17" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D18" s="10">
         <v>20</v>
@@ -1270,18 +1273,18 @@
         <v>0.8</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D19" s="10">
         <v>10</v>
@@ -1290,18 +1293,18 @@
         <v>1.2</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D20" s="10">
         <v>10</v>
@@ -1310,18 +1313,18 @@
         <v>0.87</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D21" s="10">
         <v>10</v>
@@ -1330,15 +1333,15 @@
         <v>0.62</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D22" s="10">
         <v>2</v>
@@ -1352,13 +1355,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B23" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D23" s="10">
         <v>10</v>
@@ -1367,18 +1370,18 @@
         <v>1</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D24" s="10">
         <v>10</v>
@@ -1387,18 +1390,18 @@
         <v>0.3</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B25" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D25" s="10">
         <v>10</v>
@@ -1407,18 +1410,18 @@
         <v>1</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B26" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D26" s="10">
         <v>10</v>
@@ -1427,18 +1430,18 @@
         <v>1</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B27" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D27" s="10">
         <v>10</v>
@@ -1447,18 +1450,18 @@
         <v>1</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B28" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D28" s="10">
         <v>4</v>
@@ -1467,18 +1470,18 @@
         <v>1.2</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D29" s="10">
         <v>10</v>
@@ -1487,18 +1490,18 @@
         <v>0.15</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D30" s="10">
         <v>20</v>
@@ -1507,18 +1510,18 @@
         <v>0.3</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C31" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D31" s="10">
         <v>10</v>
@@ -1527,18 +1530,18 @@
         <v>0.15</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D32" s="10">
         <v>10</v>
@@ -1547,18 +1550,18 @@
         <v>0.15</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C33" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D33" s="10">
         <v>10</v>
@@ -1567,18 +1570,18 @@
         <v>0.15</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C34" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D34" s="10">
         <v>10</v>
@@ -1587,18 +1590,18 @@
         <v>0.15</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B35" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C35" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D35" s="10">
         <v>10</v>
@@ -1607,17 +1610,28 @@
         <v>0.98</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>118</v>
+      </c>
+      <c r="D36" s="10">
+        <v>10</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C38" s="14"/>
       <c r="D38" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E38" s="12">
         <f>SUM(E2:E35)</f>
-        <v>73.350000000000023</v>
+        <v>73.490000000000023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Submitted to PCBWay for build
</commit_message>
<xml_diff>
--- a/Hardware/NFC Toy BOM.xlsx
+++ b/Hardware/NFC Toy BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="123">
   <si>
     <t>Part #</t>
   </si>
@@ -387,6 +387,12 @@
   </si>
   <si>
     <t>48-LQFP</t>
+  </si>
+  <si>
+    <t>On Order</t>
+  </si>
+  <si>
+    <t>RC1005J000CS</t>
   </si>
 </sst>
 </file>
@@ -808,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,7 +855,9 @@
       <c r="H1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="I1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -883,6 +891,9 @@
       <c r="H2" t="s">
         <v>117</v>
       </c>
+      <c r="I2" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -909,6 +920,9 @@
       <c r="H3" t="s">
         <v>117</v>
       </c>
+      <c r="I3" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -935,6 +949,9 @@
       <c r="H4" t="s">
         <v>117</v>
       </c>
+      <c r="I4" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -961,6 +978,9 @@
       <c r="H5" t="s">
         <v>117</v>
       </c>
+      <c r="I5" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
@@ -984,6 +1004,9 @@
       <c r="H6" t="s">
         <v>117</v>
       </c>
+      <c r="I6" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -1010,6 +1033,9 @@
       <c r="H7" t="s">
         <v>117</v>
       </c>
+      <c r="I7" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -1033,6 +1059,9 @@
       <c r="H8" t="s">
         <v>117</v>
       </c>
+      <c r="I8" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
@@ -1059,6 +1088,9 @@
       <c r="H9" t="s">
         <v>117</v>
       </c>
+      <c r="I9" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -1085,6 +1117,9 @@
       <c r="H10" t="s">
         <v>117</v>
       </c>
+      <c r="I10" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -1111,6 +1146,9 @@
       <c r="H11" t="s">
         <v>41</v>
       </c>
+      <c r="I11" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -1137,6 +1175,9 @@
       <c r="H12" t="s">
         <v>41</v>
       </c>
+      <c r="I12" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1160,6 +1201,9 @@
       <c r="H13" t="s">
         <v>41</v>
       </c>
+      <c r="I13" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -1183,6 +1227,9 @@
       <c r="H14" t="s">
         <v>41</v>
       </c>
+      <c r="I14" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -1206,6 +1253,9 @@
       <c r="H15" t="s">
         <v>117</v>
       </c>
+      <c r="I15" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -1229,8 +1279,11 @@
       <c r="H16" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -1255,8 +1308,11 @@
       <c r="H17" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>101</v>
       </c>
@@ -1275,8 +1331,11 @@
       <c r="F18" s="7" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>104</v>
       </c>
@@ -1295,8 +1354,11 @@
       <c r="F19" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>105</v>
       </c>
@@ -1315,8 +1377,11 @@
       <c r="F20" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>107</v>
       </c>
@@ -1335,8 +1400,11 @@
       <c r="F21" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>97</v>
       </c>
@@ -1352,8 +1420,11 @@
       <c r="F22" s="4">
         <v>1206</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>109</v>
       </c>
@@ -1372,8 +1443,11 @@
       <c r="F23" s="7" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>110</v>
       </c>
@@ -1392,8 +1466,11 @@
       <c r="F24" s="7" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>111</v>
       </c>
@@ -1412,8 +1489,11 @@
       <c r="F25" s="7" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>112</v>
       </c>
@@ -1432,8 +1512,11 @@
       <c r="F26" s="7" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>113</v>
       </c>
@@ -1452,8 +1535,11 @@
       <c r="F27" s="7" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>95</v>
       </c>
@@ -1472,8 +1558,11 @@
       <c r="F28" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>93</v>
       </c>
@@ -1492,8 +1581,11 @@
       <c r="F29" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>87</v>
       </c>
@@ -1512,8 +1604,11 @@
       <c r="F30" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>89</v>
       </c>
@@ -1532,8 +1627,11 @@
       <c r="F31" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>90</v>
       </c>
@@ -1552,8 +1650,11 @@
       <c r="F32" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>91</v>
       </c>
@@ -1572,8 +1673,11 @@
       <c r="F33" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>92</v>
       </c>
@@ -1592,8 +1696,11 @@
       <c r="F34" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>114</v>
       </c>
@@ -1612,8 +1719,17 @@
       <c r="F35" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I35" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B36" t="s">
+        <v>106</v>
+      </c>
       <c r="C36" t="s">
         <v>118</v>
       </c>
@@ -1623,8 +1739,11 @@
       <c r="F36" s="7" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I36" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C38" s="14"/>
       <c r="D38" s="1" t="s">
         <v>98</v>
@@ -1650,8 +1769,9 @@
     <hyperlink ref="A23" r:id="rId12" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/885012005010/732-7428-1-ND/5454055"/>
     <hyperlink ref="A24" r:id="rId13" display="https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM155R60J102KA01D/490-6285-1-ND/3845482"/>
     <hyperlink ref="A35" r:id="rId14" display="https://www.digikey.com/product-detail/en/susumu/RR0816P-104-D/RR08P100KDCT-ND/432772"/>
+    <hyperlink ref="A36" r:id="rId15" display="https://www.digikey.com/product-detail/en/samsung-electro-mechanics/RC1005J000CS/1276-3480-1-ND/3903583"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added J-Link adapter and 1st cut of software
</commit_message>
<xml_diff>
--- a/Hardware/NFC Toy BOM.xlsx
+++ b/Hardware/NFC Toy BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="130">
   <si>
     <t>Part #</t>
   </si>
@@ -393,6 +393,27 @@
   </si>
   <si>
     <t>RC1005J000CS</t>
+  </si>
+  <si>
+    <t>SFH11-PBPC-D05-ST-BK</t>
+  </si>
+  <si>
+    <t>10-pin plug - 0.1"</t>
+  </si>
+  <si>
+    <t>Through Hole</t>
+  </si>
+  <si>
+    <t>20021121-00010C4LF</t>
+  </si>
+  <si>
+    <t>Amphenol</t>
+  </si>
+  <si>
+    <t>10-pin header - .005"</t>
+  </si>
+  <si>
+    <t>SMT</t>
   </si>
 </sst>
 </file>
@@ -812,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1743,12 +1764,55 @@
         <v>117</v>
       </c>
     </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C37" t="s">
+        <v>124</v>
+      </c>
+      <c r="D37" s="10">
+        <v>1</v>
+      </c>
+      <c r="E37" s="12">
+        <v>0.66</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C38" s="14"/>
-      <c r="D38" s="1" t="s">
+      <c r="A38" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B38" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38" t="s">
+        <v>128</v>
+      </c>
+      <c r="D38" s="10">
+        <v>1</v>
+      </c>
+      <c r="E38" s="12">
+        <v>0.84</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="8"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C41" s="14"/>
+      <c r="D41" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E38" s="12">
+      <c r="E41" s="12">
         <f>SUM(E2:E35)</f>
         <v>73.490000000000023</v>
       </c>
@@ -1770,8 +1834,10 @@
     <hyperlink ref="A24" r:id="rId13" display="https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM155R60J102KA01D/490-6285-1-ND/3845482"/>
     <hyperlink ref="A35" r:id="rId14" display="https://www.digikey.com/product-detail/en/susumu/RR0816P-104-D/RR08P100KDCT-ND/432772"/>
     <hyperlink ref="A36" r:id="rId15" display="https://www.digikey.com/product-detail/en/samsung-electro-mechanics/RC1005J000CS/1276-3480-1-ND/3903583"/>
+    <hyperlink ref="A37" r:id="rId16" display="https://www.digikey.com/product-detail/en/sullins-connector-solutions/SFH11-PBPC-D05-ST-BK/S9194-ND/1990087"/>
+    <hyperlink ref="A38" r:id="rId17" display="https://www.digikey.com/product-detail/en/amphenol-fci/20021121-00010C4LF/609-3695-1-ND/2209147"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>